<commit_message>
mises à jour mineures
</commit_message>
<xml_diff>
--- a/sorbonne-paris-nord/SPN_ACV_TP_données.xlsx
+++ b/sorbonne-paris-nord/SPN_ACV_TP_données.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\lca-teaching\sorbonne-paris-nord\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14664C6-DE7F-4062-B2B8-1FBDCA9AE5F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60169E55-3203-4FB1-8F1F-E254E4276B3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{C508237C-FCEB-47CF-80E6-621039195DB4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{C508237C-FCEB-47CF-80E6-621039195DB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="9" r:id="rId1"/>
@@ -1288,6 +1288,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1312,8 +1314,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -13707,7 +13707,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$I$6" spid="_x0000_s1076"/>
+                  <a14:cameraTool cellRange="$I$6" spid="_x0000_s1217"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -13772,7 +13772,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$I$7" spid="_x0000_s1077"/>
+                  <a14:cameraTool cellRange="$I$7" spid="_x0000_s1218"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -13837,7 +13837,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$I$8" spid="_x0000_s1078"/>
+                  <a14:cameraTool cellRange="$I$8" spid="_x0000_s1219"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -14940,8 +14940,8 @@
   </sheetPr>
   <dimension ref="B1:AM176"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A34" zoomScale="89" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -17797,7 +17797,7 @@
       <c r="F52" s="13">
         <v>0</v>
       </c>
-      <c r="G52" s="114">
+      <c r="G52" s="106">
         <f>$F$8/100/(1-$F$9)</f>
         <v>0.19999999999999998</v>
       </c>
@@ -17904,7 +17904,7 @@
       <c r="F53" s="13">
         <v>0</v>
       </c>
-      <c r="G53" s="115">
+      <c r="G53" s="107">
         <v>0</v>
       </c>
       <c r="H53" s="2">
@@ -28058,8 +28058,8 @@
   </sheetPr>
   <dimension ref="A1:AF38"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q75" sqref="Q75"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q39" sqref="Q39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -28075,65 +28075,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="109" t="s">
+      <c r="C1" s="111" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
-      <c r="G1" s="110"/>
-      <c r="H1" s="111"/>
-      <c r="I1" s="106" t="s">
+      <c r="D1" s="112"/>
+      <c r="E1" s="112"/>
+      <c r="F1" s="112"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="108" t="s">
         <v>124</v>
       </c>
-      <c r="J1" s="106"/>
-      <c r="K1" s="106"/>
-      <c r="L1" s="106"/>
-      <c r="M1" s="106"/>
-      <c r="N1" s="106"/>
-      <c r="R1" s="106" t="s">
+      <c r="J1" s="108"/>
+      <c r="K1" s="108"/>
+      <c r="L1" s="108"/>
+      <c r="M1" s="108"/>
+      <c r="N1" s="108"/>
+      <c r="R1" s="108" t="s">
         <v>129</v>
       </c>
-      <c r="S1" s="106"/>
-      <c r="T1" s="106"/>
-      <c r="U1" s="106"/>
-      <c r="V1" s="106"/>
-      <c r="W1" s="106"/>
-      <c r="X1" s="106"/>
-      <c r="Y1" s="106" t="s">
+      <c r="S1" s="108"/>
+      <c r="T1" s="108"/>
+      <c r="U1" s="108"/>
+      <c r="V1" s="108"/>
+      <c r="W1" s="108"/>
+      <c r="X1" s="108"/>
+      <c r="Y1" s="108" t="s">
         <v>130</v>
       </c>
-      <c r="Z1" s="106"/>
-      <c r="AE1" s="106" t="s">
+      <c r="Z1" s="108"/>
+      <c r="AE1" s="108" t="s">
         <v>131</v>
       </c>
-      <c r="AF1" s="106"/>
+      <c r="AF1" s="108"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="C2" s="107" t="s">
+      <c r="C2" s="109" t="s">
         <v>129</v>
       </c>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106" t="s">
+      <c r="D2" s="108"/>
+      <c r="E2" s="108" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="106"/>
-      <c r="G2" s="106" t="s">
+      <c r="F2" s="108"/>
+      <c r="G2" s="108" t="s">
         <v>131</v>
       </c>
-      <c r="H2" s="108"/>
-      <c r="I2" s="106" t="s">
+      <c r="H2" s="110"/>
+      <c r="I2" s="108" t="s">
         <v>123</v>
       </c>
-      <c r="J2" s="106"/>
-      <c r="K2" s="106" t="s">
+      <c r="J2" s="108"/>
+      <c r="K2" s="108" t="s">
         <v>109</v>
       </c>
-      <c r="L2" s="106"/>
-      <c r="M2" s="106" t="s">
+      <c r="L2" s="108"/>
+      <c r="M2" s="108" t="s">
         <v>120</v>
       </c>
-      <c r="N2" s="106"/>
+      <c r="N2" s="108"/>
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
@@ -30460,14 +30460,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B1" s="112" t="s">
+      <c r="B1" s="114" t="s">
         <v>168</v>
       </c>
-      <c r="C1" s="112"/>
-      <c r="D1" s="113" t="s">
+      <c r="C1" s="114"/>
+      <c r="D1" s="115" t="s">
         <v>169</v>
       </c>
-      <c r="E1" s="113"/>
+      <c r="E1" s="115"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -30862,7 +30862,7 @@
   <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>